<commit_message>
Meer data, meer opgekuist
</commit_message>
<xml_diff>
--- a/2016Robbertmetingen.xlsx
+++ b/2016Robbertmetingen.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Kalibratiemetingen" sheetId="1" r:id="rId1"/>
-    <sheet name="Impedantiemeter" sheetId="2" r:id="rId2"/>
-    <sheet name="PeriodeTest" sheetId="3" r:id="rId3"/>
+    <sheet name="Blad1" sheetId="4" r:id="rId2"/>
+    <sheet name="Impedantiemeter" sheetId="2" r:id="rId3"/>
+    <sheet name="PeriodeTest" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="77">
   <si>
     <t>Sample nummer</t>
   </si>
@@ -95,15 +96,6 @@
     <t>Top B shunt µs</t>
   </si>
   <si>
-    <t>Periode</t>
-  </si>
-  <si>
-    <t>Faseverschil</t>
-  </si>
-  <si>
-    <t>Verhouding</t>
-  </si>
-  <si>
     <t>Gain resistance</t>
   </si>
   <si>
@@ -135,6 +127,132 @@
   </si>
   <si>
     <t>afwijking in percent tov leeg</t>
+  </si>
+  <si>
+    <t>Gemiddele periode</t>
+  </si>
+  <si>
+    <t>nxt pk B</t>
+  </si>
+  <si>
+    <t>nxt pk A</t>
+  </si>
+  <si>
+    <t>Periode A</t>
+  </si>
+  <si>
+    <t>Periode B</t>
+  </si>
+  <si>
+    <t>Faseverschil 1 (°)</t>
+  </si>
+  <si>
+    <t>Faseverschil 2 (°)</t>
+  </si>
+  <si>
+    <t>freq awg</t>
+  </si>
+  <si>
+    <t>AWG</t>
+  </si>
+  <si>
+    <t>9V</t>
+  </si>
+  <si>
+    <t>Uitleg:</t>
+  </si>
+  <si>
+    <t>Top is telkens waar de piek van dat kanaal voorkomt. (in microseconden). Zo kan de faseverschuiving bepaald worden. Deze waarden zijn gemeten met de picoscope. Van elk kanaal worden 2 opeenvolgende pieken bepaald. Hieruit wordt de periode tweemaal berekend, de gemiddelde periode en ook tweemaal het faseverschil. De in te stellen parameters op de PCB worden ook meegegeven, de gebruikte toestellen en frequentie.</t>
+  </si>
+  <si>
+    <t>Hier worden een aantal materialen in de humidity sensor gestoken, om te kijken of het aantal periodicos veranderen. Dit blijkt het geval te zijn. Wel moet in het achterhoofd gehouden worden dat de lege meting eraf getrokken wordt, en dat een verschil van 700 flanken overeen komt met een verschil van ongeveer 1% humidity</t>
+  </si>
+  <si>
+    <t>heeft geregend</t>
+  </si>
+  <si>
+    <t>Periodicos lege meters</t>
+  </si>
+  <si>
+    <t>3,0-7</t>
+  </si>
+  <si>
+    <t>3,0-18</t>
+  </si>
+  <si>
+    <t>opmerking</t>
+  </si>
+  <si>
+    <t>battery 4,8v</t>
+  </si>
+  <si>
+    <t>knoppen zijn belachelijk slecht</t>
+  </si>
+  <si>
+    <t>batterij net vervangen, werkte niet meer</t>
+  </si>
+  <si>
+    <t>3,0-12</t>
+  </si>
+  <si>
+    <t>3,0-3</t>
+  </si>
+  <si>
+    <t>3,0-8</t>
+  </si>
+  <si>
+    <t>dat consistency</t>
+  </si>
+  <si>
+    <t>3,0-1</t>
+  </si>
+  <si>
+    <t>3,0-10</t>
+  </si>
+  <si>
+    <t>3,0-11</t>
+  </si>
+  <si>
+    <t>3,0-14</t>
+  </si>
+  <si>
+    <t>3,0-13</t>
+  </si>
+  <si>
+    <t>3,0-5</t>
+  </si>
+  <si>
+    <t>opmerking 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">op 08/07 heeft het heel veel geregend. </t>
+  </si>
+  <si>
+    <t>3,0-6</t>
+  </si>
+  <si>
+    <t>geeft heel wisselende waarden tussen 21k en 23k, stabiliseert na een tijd naar 21k</t>
+  </si>
+  <si>
+    <t>3,0-16</t>
+  </si>
+  <si>
+    <t>staat oude/andere software op</t>
+  </si>
+  <si>
+    <t>2,3-1</t>
+  </si>
+  <si>
+    <t>staat oude/andere software op, batterij 6,4V</t>
+  </si>
+  <si>
+    <t>3,0-17</t>
+  </si>
+  <si>
+    <t>3,0-15</t>
+  </si>
+  <si>
+    <t>3,0-4</t>
   </si>
 </sst>
 </file>
@@ -144,7 +262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -173,8 +291,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,18 +309,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -202,23 +352,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Verklarende tekst" xfId="1" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -231,6 +442,1196 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="nl-BE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Kalibratiemetingen!$B$4:$B$50000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49997"/>
+                <c:pt idx="0">
+                  <c:v>17.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Kalibratiemetingen!$F$4:$F$50000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49997"/>
+                <c:pt idx="0">
+                  <c:v>6274</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5635</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4577</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3728</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5617</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5081</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5546</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5379</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4834</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5908</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3614</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3713</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4436</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3546</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5720</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4329</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3097</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5232</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2723</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3339</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3076</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CB0E-428C-97C1-A82916D913E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="307533840"/>
+        <c:axId val="307534496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="307533840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-BE" sz="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Gehaka</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-BE" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> humidity</a:t>
+                </a:r>
+                <a:endParaRPr lang="nl-BE" sz="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-BE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="307534496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="307534496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-BE" sz="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Periodicos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-BE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="307533840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-BE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,493 +1931,574 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375"/>
-    <col min="2" max="2" width="17.140625"/>
-    <col min="3" max="3" width="14.140625"/>
-    <col min="4" max="4" width="16.42578125"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11"/>
-    <col min="8" max="8" width="18.140625"/>
-    <col min="9" max="9" width="14.5703125"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="8"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375"/>
     <col min="11" max="11" width="8.5703125"/>
-    <col min="12" max="12" width="24.140625"/>
-    <col min="13" max="1025" width="8.5703125"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>COUNT(A$4:A$65000)</f>
+        <v>22</v>
+      </c>
+      <c r="B1" s="12">
+        <f>COUNT(B$4:B$65000)</f>
+        <v>24</v>
+      </c>
+      <c r="C1" s="12">
+        <f>COUNT(C$4:C$65000)</f>
+        <v>12</v>
+      </c>
+      <c r="D1" s="12">
+        <f t="shared" ref="D1:N1" si="0">COUNT(D$4:D$65000)</f>
+        <v>0</v>
+      </c>
+      <c r="E1" s="12">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="F1" s="12">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="G1" s="12">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="M1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="20">
         <v>8703</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="21">
         <v>17.8</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="E4" s="5">
+      <c r="C4" s="22"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="23">
         <v>21629</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="24">
         <v>6274</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="23">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="20">
         <v>729</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="25">
         <v>42551</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="20">
         <v>8705</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="21">
         <v>14.6</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="E5" s="5">
+      <c r="C5" s="22"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="23">
         <v>21696</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="24">
         <v>5635</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="23">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="20">
         <v>729</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="25">
         <v>42551</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="20">
         <v>8667</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="21">
         <v>13.7</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="E6" s="5">
+      <c r="C6" s="22"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="23">
         <v>21709</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="24">
         <v>4577</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="23">
         <v>31</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="20">
         <v>729</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="25">
         <v>42551</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="20">
         <v>8708</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="21">
         <v>12</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="E7" s="5">
+      <c r="C7" s="22"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="23">
         <v>21719</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="24">
         <v>3728</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="23">
         <v>31</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="20">
         <v>729</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="25">
         <v>42551</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="20">
         <v>8717</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="21">
         <v>14.6</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="E8" s="5">
+      <c r="C8" s="22"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="23">
         <v>21686</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="24">
         <v>5617</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="23">
         <v>33</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="20">
         <v>729</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="25">
         <v>42551</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21">
         <v>16.100000000000001</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="E9" s="5">
+      <c r="C9" s="22"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="23">
         <v>21647</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="24">
         <v>5908</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="23">
         <v>33</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="20">
         <v>729</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="25">
         <v>42551</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21">
         <v>13.9</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="E10" s="5">
+      <c r="C10" s="22"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="23">
         <v>21646</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="24">
         <v>5081</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="23">
         <v>32</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="20">
         <v>729</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="25">
         <v>42551</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="20">
         <v>8723</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="21">
         <v>12</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="E11" s="5">
+      <c r="C11" s="22"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="23">
         <v>21682</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="24">
         <v>3935</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="23">
         <v>33</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="20">
         <v>729</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="25">
         <v>42551</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="20">
         <v>8649</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="21">
         <v>14.8</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="E12" s="5">
+      <c r="C12" s="22"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="23">
         <v>21538</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="24">
         <v>5546</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="23">
         <v>31</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="20">
         <v>729</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="25">
         <v>42551</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="20">
         <v>8647</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="21">
         <v>13.7</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="E13" s="5">
+      <c r="C13" s="22"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="23">
         <v>21548</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="24">
         <v>5379</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="23">
         <v>31</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="20">
         <v>729</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="25">
         <v>42551</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="20">
         <v>123</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="21">
         <v>12.1</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="E14" s="5">
+      <c r="C14" s="22"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="23">
         <v>21572</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="24">
         <v>4834</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="23">
         <v>31</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="20">
         <v>729</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="25">
         <v>42551</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="20" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1024,17 +2506,17 @@
       <c r="A15">
         <v>121</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="7">
         <v>15.1</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="E15" s="5">
+      <c r="C15" s="9"/>
+      <c r="E15" s="10">
         <v>21521</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="11">
         <v>5908</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="10">
         <v>31</v>
       </c>
       <c r="H15" t="s">
@@ -1049,7 +2531,7 @@
       <c r="K15" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="1">
         <v>42551</v>
       </c>
       <c r="M15" t="s">
@@ -1063,29 +2545,29 @@
       <c r="A16">
         <v>8892</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="7">
         <v>11.2</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="9">
         <v>31.3</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="10">
         <v>22250</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="11">
         <v>3614</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="10">
         <v>25</v>
       </c>
       <c r="H16" t="s">
         <v>14</v>
       </c>
       <c r="I16">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="J16" t="s">
         <v>15</v>
@@ -1093,7 +2575,7 @@
       <c r="K16" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="1">
         <v>42556</v>
       </c>
       <c r="M16" t="s">
@@ -1104,29 +2586,29 @@
       <c r="A17">
         <v>175</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="7">
         <v>11.2</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="9">
         <v>31.3</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="10">
         <v>22353</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="11">
         <v>3713</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="10">
         <v>26</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
       </c>
       <c r="I17">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="J17" t="s">
         <v>15</v>
@@ -1134,7 +2616,7 @@
       <c r="K17" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L17" s="1">
         <v>42556</v>
       </c>
       <c r="M17" t="s">
@@ -1145,29 +2627,29 @@
       <c r="A18">
         <v>212</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="7">
         <v>14.5</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="9">
         <v>31.5</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="10">
         <v>22372</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="11">
         <v>4436</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="10">
         <v>26</v>
       </c>
       <c r="H18" t="s">
         <v>14</v>
       </c>
       <c r="I18">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="J18" t="s">
         <v>15</v>
@@ -1175,7 +2657,7 @@
       <c r="K18" t="s">
         <v>16</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="1">
         <v>42556</v>
       </c>
       <c r="M18" t="s">
@@ -1186,29 +2668,29 @@
       <c r="A19">
         <v>173</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="6">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="8">
         <v>31.4</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="8">
         <v>22366</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="6">
         <v>1680</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="8">
         <v>26</v>
       </c>
       <c r="H19" t="s">
         <v>14</v>
       </c>
       <c r="I19">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="J19" t="s">
         <v>15</v>
@@ -1216,7 +2698,7 @@
       <c r="K19" t="s">
         <v>16</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="1">
         <v>42556</v>
       </c>
       <c r="M19" t="s">
@@ -1227,29 +2709,29 @@
       <c r="A20">
         <v>174</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="6">
         <v>11</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="8">
         <v>31.3</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="8">
         <v>22367</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="6">
         <v>3546</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="8">
         <v>26</v>
       </c>
       <c r="H20" t="s">
         <v>14</v>
       </c>
       <c r="I20">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="J20" t="s">
         <v>15</v>
@@ -1257,7 +2739,7 @@
       <c r="K20" t="s">
         <v>16</v>
       </c>
-      <c r="L20" s="6">
+      <c r="L20" s="1">
         <v>42556</v>
       </c>
       <c r="M20" t="s">
@@ -1268,29 +2750,29 @@
       <c r="A21">
         <v>8894</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="6">
         <v>13.8</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="8">
         <v>31.8</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="8">
         <v>22306</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="6">
         <v>5720</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="8">
         <v>26</v>
       </c>
       <c r="H21" t="s">
         <v>14</v>
       </c>
       <c r="I21">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="J21" t="s">
         <v>15</v>
@@ -1298,7 +2780,7 @@
       <c r="K21" t="s">
         <v>16</v>
       </c>
-      <c r="L21" s="6">
+      <c r="L21" s="1">
         <v>42556</v>
       </c>
       <c r="M21" t="s">
@@ -1309,29 +2791,29 @@
       <c r="A22">
         <v>8895</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="6">
         <v>11.8</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="8">
         <v>31.7</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="8">
         <v>22306</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="6">
         <v>4329</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="8">
         <v>26</v>
       </c>
       <c r="H22" t="s">
         <v>14</v>
       </c>
       <c r="I22">
-        <v>736</v>
+        <v>729</v>
       </c>
       <c r="J22" t="s">
         <v>15</v>
@@ -1339,7 +2821,7 @@
       <c r="K22" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="6">
+      <c r="L22" s="1">
         <v>42556</v>
       </c>
       <c r="M22" t="s">
@@ -1350,29 +2832,29 @@
       <c r="A23">
         <v>8840</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="6">
         <v>10.8</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="8">
         <v>31.6</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="8">
         <v>22203</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="6">
         <v>3097</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="8">
         <v>25</v>
       </c>
       <c r="H23" t="s">
         <v>14</v>
       </c>
       <c r="I23">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="J23" t="s">
         <v>15</v>
@@ -1380,7 +2862,7 @@
       <c r="K23" t="s">
         <v>16</v>
       </c>
-      <c r="L23" s="6">
+      <c r="L23" s="1">
         <v>42556</v>
       </c>
       <c r="M23" t="s">
@@ -1391,29 +2873,29 @@
       <c r="A24">
         <v>8850</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="6">
         <v>13.4</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="8">
         <v>31.4</v>
       </c>
       <c r="D24" t="s">
         <v>21</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="8">
         <v>22217</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="6">
         <v>5232</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="8">
         <v>25</v>
       </c>
       <c r="H24" t="s">
         <v>14</v>
       </c>
       <c r="I24">
-        <v>738</v>
+        <v>729</v>
       </c>
       <c r="J24" t="s">
         <v>15</v>
@@ -1421,7 +2903,7 @@
       <c r="K24" t="s">
         <v>16</v>
       </c>
-      <c r="L24" s="6">
+      <c r="L24" s="1">
         <v>42556</v>
       </c>
       <c r="M24" t="s">
@@ -1432,29 +2914,29 @@
       <c r="A25">
         <v>8852</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="6">
         <v>10.8</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="8">
         <v>31.5</v>
       </c>
       <c r="D25" t="s">
         <v>21</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="8">
         <v>22215</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="6">
         <v>2723</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="8">
         <v>25</v>
       </c>
       <c r="H25" t="s">
         <v>14</v>
       </c>
       <c r="I25">
-        <v>739</v>
+        <v>729</v>
       </c>
       <c r="J25" t="s">
         <v>15</v>
@@ -1462,7 +2944,7 @@
       <c r="K25" t="s">
         <v>16</v>
       </c>
-      <c r="L25" s="6">
+      <c r="L25" s="1">
         <v>42556</v>
       </c>
       <c r="M25" t="s">
@@ -1473,29 +2955,29 @@
       <c r="A26">
         <v>8851</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="6">
         <v>10.8</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="8">
         <v>31.5</v>
       </c>
       <c r="D26" t="s">
         <v>21</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="8">
         <v>22216</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="6">
         <v>3339</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="8">
         <v>26</v>
       </c>
       <c r="H26" t="s">
         <v>14</v>
       </c>
       <c r="I26">
-        <v>740</v>
+        <v>729</v>
       </c>
       <c r="J26" t="s">
         <v>15</v>
@@ -1503,7 +2985,7 @@
       <c r="K26" t="s">
         <v>16</v>
       </c>
-      <c r="L26" s="6">
+      <c r="L26" s="1">
         <v>42556</v>
       </c>
       <c r="M26" t="s">
@@ -1514,29 +2996,29 @@
       <c r="A27">
         <v>8858</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="6">
         <v>10.8</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="8">
         <v>31.6</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="8">
         <v>22212</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="6">
         <v>3076</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="8">
         <v>26</v>
       </c>
       <c r="H27" t="s">
         <v>14</v>
       </c>
       <c r="I27">
-        <v>741</v>
+        <v>729</v>
       </c>
       <c r="J27" t="s">
         <v>15</v>
@@ -1544,7 +3026,7 @@
       <c r="K27" t="s">
         <v>16</v>
       </c>
-      <c r="L27" s="6">
+      <c r="L27" s="1">
         <v>42556</v>
       </c>
       <c r="M27" t="s">
@@ -1552,81 +3034,1083 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L28" s="6">
-        <v>42556</v>
+      <c r="D28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28">
+        <v>729</v>
+      </c>
+      <c r="J28" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" s="1">
+        <v>42558</v>
       </c>
       <c r="M28" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="26">
+        <v>42559</v>
+      </c>
+      <c r="C3" s="26">
+        <v>42559</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>24888</v>
+      </c>
+      <c r="C4">
+        <v>24933</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>16469</v>
+      </c>
+      <c r="C5">
+        <v>16482</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>17109</v>
+      </c>
+      <c r="C6">
+        <v>17083</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>21039</v>
+      </c>
+      <c r="C7">
+        <v>21075</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8">
+        <v>17225</v>
+      </c>
+      <c r="C8">
+        <v>17237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>20472</v>
+      </c>
+      <c r="C9">
+        <v>20472</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>17155</v>
+      </c>
+      <c r="C10">
+        <v>17053</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
+        <v>23131</v>
+      </c>
+      <c r="C11">
+        <v>23142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12">
+        <v>20786</v>
+      </c>
+      <c r="C12">
+        <v>20800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13">
+        <v>23576</v>
+      </c>
+      <c r="C13">
+        <v>23584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14">
+        <v>16736</v>
+      </c>
+      <c r="C14">
+        <v>16740</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <v>23538</v>
+      </c>
+      <c r="C15">
+        <v>21597</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16">
+        <v>16855</v>
+      </c>
+      <c r="C16">
+        <v>16863</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17">
+        <v>17667</v>
+      </c>
+      <c r="C17">
+        <v>17660</v>
+      </c>
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18">
+        <v>20042</v>
+      </c>
+      <c r="C18">
+        <v>20108</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19">
+        <v>20633</v>
+      </c>
+      <c r="C19">
+        <v>20621</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="K3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="L3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="M3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>30</v>
+      <c r="N3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>617</v>
+      </c>
+      <c r="B4">
+        <v>705</v>
+      </c>
+      <c r="C4">
+        <v>956</v>
+      </c>
+      <c r="D4">
+        <v>1048</v>
+      </c>
+      <c r="E4">
+        <f>C4-A4</f>
+        <v>339</v>
+      </c>
+      <c r="F4">
+        <f>D4-B4</f>
+        <v>343</v>
+      </c>
+      <c r="G4">
+        <f>AVERAGE(E4:F4)</f>
+        <v>341</v>
+      </c>
+      <c r="H4">
+        <f>((B4-A4)/G4)*360</f>
+        <v>92.903225806451616</v>
+      </c>
+      <c r="I4">
+        <f>(D4-C4)/G4*360</f>
+        <v>97.126099706744867</v>
+      </c>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>680</v>
+      </c>
+      <c r="B5">
+        <v>826</v>
+      </c>
+      <c r="C5">
+        <v>1184</v>
+      </c>
+      <c r="D5">
+        <v>1324</v>
+      </c>
+      <c r="E5">
+        <f>C5-A5</f>
+        <v>504</v>
+      </c>
+      <c r="F5">
+        <f>D5-B5</f>
+        <v>498</v>
+      </c>
+      <c r="G5">
+        <f>AVERAGE(E5:F5)</f>
+        <v>501</v>
+      </c>
+      <c r="H5">
+        <f>((B5-A5)/G5)*360</f>
+        <v>104.91017964071855</v>
+      </c>
+      <c r="I5">
+        <f>(D5-C5)/G5*360</f>
+        <v>100.59880239520957</v>
+      </c>
+      <c r="L5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1170</v>
+      </c>
+      <c r="B6">
+        <v>1508</v>
+      </c>
+      <c r="C6">
+        <v>2166</v>
+      </c>
+      <c r="D6">
+        <v>2514</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E31" si="0">C6-A6</f>
+        <v>996</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F31" si="1">D6-B6</f>
+        <v>1006</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G31" si="2">AVERAGE(E6:F6)</f>
+        <v>1001</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H31" si="3">((B6-A6)/G6)*360</f>
+        <v>121.55844155844156</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I31" si="4">(D6-C6)/G6*360</f>
+        <v>125.15484515484515</v>
+      </c>
+      <c r="L6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8050</v>
+      </c>
+      <c r="B7">
+        <v>13000</v>
+      </c>
+      <c r="C7">
+        <v>18200</v>
+      </c>
+      <c r="D7">
+        <v>23000</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>10150</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>10075</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>176.87344913151364</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>171.5136476426799</v>
+      </c>
+      <c r="N7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H11" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H14" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H16" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H17" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H18" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H19" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H20" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H21" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H23" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H24" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I24" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H25" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I26" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H27" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I27" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H28" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H29" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H30" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I30" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H31" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,17 +4120,31 @@
     <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G4" s="7" t="s">
-        <v>36</v>
+      <c r="G4" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
+      <c r="A5" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B5">
         <v>21089</v>
@@ -1673,8 +4171,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>34</v>
+      <c r="A6" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B6">
         <v>22307</v>
@@ -1701,8 +4199,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
+      <c r="A7" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B7">
         <v>21307</v>
@@ -1729,8 +4227,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>33</v>
+      <c r="A8" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B8">
         <v>21084</v>
@@ -1757,8 +4255,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>31</v>
+      <c r="A9" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B9">
         <v>21034</v>
@@ -1775,7 +4273,7 @@
       <c r="F9">
         <v>21062</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="3">
         <f>AVERAGE(B9:F9)</f>
         <v>21050.6</v>
       </c>
@@ -1784,7 +4282,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
consistente metingen met Freek
</commit_message>
<xml_diff>
--- a/2016Robbertmetingen.xlsx
+++ b/2016Robbertmetingen.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Kalibratiemetingen" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad1" sheetId="4" r:id="rId2"/>
+    <sheet name="LegePeriodicos" sheetId="4" r:id="rId2"/>
     <sheet name="Impedantiemeter" sheetId="2" r:id="rId3"/>
     <sheet name="PeriodeTest" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="76">
   <si>
     <t>Sample nummer</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>Hier worden een aantal materialen in de humidity sensor gestoken, om te kijken of het aantal periodicos veranderen. Dit blijkt het geval te zijn. Wel moet in het achterhoofd gehouden worden dat de lege meting eraf getrokken wordt, en dat een verschil van 700 flanken overeen komt met een verschil van ongeveer 1% humidity</t>
-  </si>
-  <si>
-    <t>heeft geregend</t>
   </si>
   <si>
     <t>Periodicos lege meters</t>
@@ -394,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -426,6 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -625,6 +623,39 @@
                 <c:pt idx="23">
                   <c:v>10.8</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>14.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11.4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -705,6 +736,36 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>3076</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5479</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5222</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4905</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4857</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4007</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5068</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5386</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5589</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4876</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1932,10 +1993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,7 +2012,7 @@
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375"/>
     <col min="11" max="11" width="8.5703125"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="1025" width="8.5703125"/>
@@ -1960,15 +2021,15 @@
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>COUNT(A$4:A$65000)</f>
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B1" s="10">
         <f>COUNT(B$4:B$65000)</f>
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C1" s="10">
         <f>COUNT(C$4:C$65000)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D1" s="10">
         <f t="shared" ref="D1:N1" si="0">COUNT(D$4:D$65000)</f>
@@ -1976,15 +2037,15 @@
       </c>
       <c r="E1" s="10">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F1" s="10">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G1" s="10">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="H1">
         <f t="shared" si="0"/>
@@ -1992,7 +2053,7 @@
       </c>
       <c r="I1">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J1">
         <f t="shared" si="0"/>
@@ -2004,7 +2065,7 @@
       </c>
       <c r="L1">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="M1">
         <f t="shared" si="0"/>
@@ -3035,8 +3096,26 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>9200</v>
+      </c>
+      <c r="B28" s="4">
+        <v>14.1</v>
+      </c>
+      <c r="C28" s="6">
+        <v>28.7</v>
+      </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="E28" s="6">
+        <v>21798</v>
+      </c>
+      <c r="F28" s="4">
+        <v>5479</v>
+      </c>
+      <c r="G28" s="6">
+        <v>29</v>
       </c>
       <c r="H28" t="s">
         <v>14</v>
@@ -3051,10 +3130,366 @@
         <v>16</v>
       </c>
       <c r="L28" s="1">
-        <v>42558</v>
+        <v>42562</v>
       </c>
       <c r="M28" t="s">
-        <v>48</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9201</v>
+      </c>
+      <c r="B29" s="4">
+        <v>13.7</v>
+      </c>
+      <c r="C29" s="6">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="6">
+        <v>21874</v>
+      </c>
+      <c r="F29" s="4">
+        <v>5222</v>
+      </c>
+      <c r="G29" s="6">
+        <v>29</v>
+      </c>
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29">
+        <v>729</v>
+      </c>
+      <c r="J29" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" s="27">
+        <v>42562</v>
+      </c>
+      <c r="M29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9199</v>
+      </c>
+      <c r="B30" s="4">
+        <v>13.1</v>
+      </c>
+      <c r="C30" s="6">
+        <v>28.5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="6">
+        <v>21900</v>
+      </c>
+      <c r="F30" s="4">
+        <v>4905</v>
+      </c>
+      <c r="G30" s="6">
+        <v>29</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30">
+        <v>729</v>
+      </c>
+      <c r="J30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" s="27">
+        <v>42562</v>
+      </c>
+      <c r="M30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>14.3</v>
+      </c>
+      <c r="C31" s="6">
+        <v>28.5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>75</v>
+      </c>
+      <c r="H31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31">
+        <v>729</v>
+      </c>
+      <c r="J31" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" s="27">
+        <v>42562</v>
+      </c>
+      <c r="M31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>9192</v>
+      </c>
+      <c r="B32" s="4">
+        <v>12.6</v>
+      </c>
+      <c r="C32" s="6">
+        <v>28.1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="6">
+        <v>21962</v>
+      </c>
+      <c r="F32" s="4">
+        <v>4857</v>
+      </c>
+      <c r="G32" s="6">
+        <v>30</v>
+      </c>
+      <c r="H32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32">
+        <v>729</v>
+      </c>
+      <c r="J32" t="s">
+        <v>15</v>
+      </c>
+      <c r="K32" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" s="27">
+        <v>42562</v>
+      </c>
+      <c r="M32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>9165</v>
+      </c>
+      <c r="B33" s="4">
+        <v>11.8</v>
+      </c>
+      <c r="C33" s="6">
+        <v>27.8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="6">
+        <v>21987</v>
+      </c>
+      <c r="F33" s="4">
+        <v>4007</v>
+      </c>
+      <c r="G33" s="6">
+        <v>30</v>
+      </c>
+      <c r="H33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33">
+        <v>729</v>
+      </c>
+      <c r="J33" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="27">
+        <v>42562</v>
+      </c>
+      <c r="M33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>9162</v>
+      </c>
+      <c r="B34" s="4">
+        <v>13.1</v>
+      </c>
+      <c r="C34" s="6">
+        <v>27.5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="6">
+        <v>22004</v>
+      </c>
+      <c r="F34" s="4">
+        <v>5068</v>
+      </c>
+      <c r="G34" s="6">
+        <v>30</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34">
+        <v>729</v>
+      </c>
+      <c r="J34" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" s="27">
+        <v>42562</v>
+      </c>
+      <c r="M34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>9163</v>
+      </c>
+      <c r="B35" s="4">
+        <v>13.1</v>
+      </c>
+      <c r="C35" s="6">
+        <v>27.6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" s="6">
+        <v>22009</v>
+      </c>
+      <c r="F35" s="4">
+        <v>5386</v>
+      </c>
+      <c r="G35" s="6">
+        <v>30</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35">
+        <v>729</v>
+      </c>
+      <c r="J35" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" t="s">
+        <v>16</v>
+      </c>
+      <c r="L35" s="27">
+        <v>42562</v>
+      </c>
+      <c r="M35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>9164</v>
+      </c>
+      <c r="B36" s="4">
+        <v>13.9</v>
+      </c>
+      <c r="C36" s="6">
+        <v>27.5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" s="6">
+        <v>22016</v>
+      </c>
+      <c r="F36" s="4">
+        <v>5589</v>
+      </c>
+      <c r="G36" s="6">
+        <v>30</v>
+      </c>
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36">
+        <v>729</v>
+      </c>
+      <c r="J36" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" t="s">
+        <v>16</v>
+      </c>
+      <c r="L36" s="27">
+        <v>42562</v>
+      </c>
+      <c r="M36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>195</v>
+      </c>
+      <c r="B37" s="4">
+        <v>12.8</v>
+      </c>
+      <c r="C37" s="6">
+        <v>27.5</v>
+      </c>
+      <c r="E37" s="6">
+        <v>22050</v>
+      </c>
+      <c r="F37" s="4">
+        <v>4876</v>
+      </c>
+      <c r="G37" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>8932</v>
+      </c>
+      <c r="B38" s="4">
+        <v>11.4</v>
+      </c>
+      <c r="C38" s="6">
+        <v>27.7</v>
+      </c>
+      <c r="E38" s="6">
+        <v>21987</v>
+      </c>
+      <c r="F38" s="4">
+        <v>3899</v>
+      </c>
+      <c r="G38" s="6">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3069,7 +3504,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3082,7 +3517,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3097,15 +3532,15 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <v>24888</v>
@@ -3114,15 +3549,15 @@
         <v>24933</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>16469</v>
@@ -3131,12 +3566,12 @@
         <v>16482</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>17109</v>
@@ -3145,12 +3580,12 @@
         <v>17083</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>21039</v>
@@ -3161,7 +3596,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8">
         <v>17225</v>
@@ -3172,7 +3607,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>20472</v>
@@ -3181,12 +3616,12 @@
         <v>20472</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10">
         <v>17155</v>
@@ -3197,7 +3632,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11">
         <v>23131</v>
@@ -3208,7 +3643,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12">
         <v>20786</v>
@@ -3219,7 +3654,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13">
         <v>23576</v>
@@ -3230,7 +3665,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14">
         <v>16736</v>
@@ -3239,12 +3674,12 @@
         <v>16740</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15">
         <v>23538</v>
@@ -3253,12 +3688,12 @@
         <v>21597</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16">
         <v>16855</v>
@@ -3267,12 +3702,12 @@
         <v>16863</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17">
         <v>17667</v>
@@ -3281,12 +3716,12 @@
         <v>17660</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18">
         <v>20042</v>
@@ -3295,12 +3730,12 @@
         <v>20108</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19">
         <v>20633</v>
@@ -3318,7 +3753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>